<commit_message>
added Business rules for Work Number, Self Employment Certification
</commit_message>
<xml_diff>
--- a/Classificationresults.xlsx
+++ b/Classificationresults.xlsx
@@ -31,10 +31,10 @@
     <x:t>BucketName</x:t>
   </x:si>
   <x:si>
-    <x:t>Unit 601_Upload1.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page1.jpg</x:t>
+    <x:t>Unit 623_Upload1.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page1.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>ICW (Income Calculation Worksheet)</x:t>
@@ -43,7 +43,7 @@
     <x:t>Certifications</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page2.jpg</x:t>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page2.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>AZ Income Limit Table</x:t>
@@ -52,7 +52,7 @@
     <x:t>File Checklist</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page3.jpg</x:t>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page3.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>Application Summary</x:t>
@@ -61,31 +61,70 @@
     <x:t>Applications</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page4.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page5.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page6.jpg</x:t>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page4.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page5.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page6.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>Member Information Document Form</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload1Page7.jpg</x:t>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload1Page7.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>Income &amp; Asset Questionnaire</x:t>
   </x:si>
   <x:si>
-    <x:t>Unit 601_Upload2.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page1.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page2.jpg</x:t>
+    <x:t>Unit 623_Upload2.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page2.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page3.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page4.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Housing History Disclosure</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Other</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page5.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Emergency Contact Form</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page6.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Self Certification of Non-Employment Form</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Income</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload2Page7.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Unit 623_Upload3.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload3Page1.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload3Page2.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>Asset Self Certification Form</x:t>
@@ -94,46 +133,13 @@
     <x:t>Assets</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page3.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page4.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Housing History Disclosure</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Other</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page5.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Exact Day Calculator for Income</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Income</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page6.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Earnings Statement or Verification of Employment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload2Page7.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unit 601_Upload3.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page1.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page2.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page3.jpg</x:t>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload3Page3.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Unit 623_Upload4.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload4Page1.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>Student Certification Form</x:t>
@@ -142,61 +148,28 @@
     <x:t>Student Status</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page4.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page5.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page6.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Family Composition</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload3Page7.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Certifications </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Unit 601_Upload4.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page1.jpg</x:t>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload4Page2.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Screening Documents</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Property Management Documents</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload4Page3.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload4Page4.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\harika.malyala\Documents\AZApplicationReview\PDFs\Unit 623\Unit 623_Upload4Page5.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>VAWA Acknowledgement of Receipt</x:t>
   </x:si>
   <x:si>
     <x:t>VAWA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page2.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Screening Documents</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Property Management Documents</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page3.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page4.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page5.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page6.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>C:\Temp\Unit 601\Unit 601_Upload4Page7.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Emergency Contact Form</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -547,7 +520,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E29"/>
+  <x:dimension ref="A1:E23"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -717,10 +690,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
@@ -728,7 +701,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C11" s="0">
         <x:v>3</x:v>
@@ -745,16 +718,16 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C12" s="0">
         <x:v>4</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
@@ -762,16 +735,16 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C13" s="0">
         <x:v>5</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
@@ -779,13 +752,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C14" s="0">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
         <x:v>32</x:v>
@@ -796,13 +769,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C15" s="0">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
         <x:v>32</x:v>
@@ -810,16 +783,16 @@
     </x:row>
     <x:row r="16" spans="1:5">
       <x:c r="A16" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C16" s="0">
         <x:v>1</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
         <x:v>32</x:v>
@@ -827,24 +800,24 @@
     </x:row>
     <x:row r="17" spans="1:5">
       <x:c r="A17" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
         <x:v>36</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>38</x:v>
       </x:c>
       <x:c r="C17" s="0">
         <x:v>2</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>39</x:v>
@@ -853,197 +826,95 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
       <x:c r="A19" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C19" s="0">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="C19" s="0">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
       <x:c r="A20" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C20" s="0">
-        <x:v>5</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
       <x:c r="A21" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C21" s="0">
-        <x:v>6</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
       <x:c r="A22" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C22" s="0">
-        <x:v>7</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
       <x:c r="A23" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
       <x:c r="C23" s="0">
-        <x:v>1</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
         <x:v>51</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:5">
-      <x:c r="A24" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="C24" s="0">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D24" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E24" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:5">
-      <x:c r="A25" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="C25" s="0">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="D25" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E25" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:5">
-      <x:c r="A26" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="C26" s="0">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E26" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:5">
-      <x:c r="A27" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="C27" s="0">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E27" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5">
-      <x:c r="A28" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B28" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="C28" s="0">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E28" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:5">
-      <x:c r="A29" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="C29" s="0">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="E29" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>